<commit_message>
Sankey Diagrams, Charts, & Data
</commit_message>
<xml_diff>
--- a/analyses/team07/quinn-p-mchugh/Drug Deaths Philadelphia v.s. Nationwide.xlsx
+++ b/analyses/team07/quinn-p-mchugh/Drug Deaths Philadelphia v.s. Nationwide.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>Philadelphia</t>
   </si>
@@ -30,7 +30,10 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Found using Linear Interpolation</t>
+    <t>Estimated using Linear Interpolation</t>
+  </si>
+  <si>
+    <t>Philadelphia / Nationwide</t>
   </si>
 </sst>
 </file>
@@ -117,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -140,6 +143,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -376,11 +385,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="245634176"/>
-        <c:axId val="266673536"/>
+        <c:axId val="170888576"/>
+        <c:axId val="170894464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="245634176"/>
+        <c:axId val="170888576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -390,12 +399,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266673536"/>
+        <c:crossAx val="170894464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="266673536"/>
+        <c:axId val="170894464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -406,7 +415,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="245634176"/>
+        <c:crossAx val="170888576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -634,11 +643,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="190526208"/>
-        <c:axId val="190554112"/>
+        <c:axId val="171321216"/>
+        <c:axId val="171322752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="190526208"/>
+        <c:axId val="171321216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -648,12 +657,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190554112"/>
+        <c:crossAx val="171322752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="190554112"/>
+        <c:axId val="171322752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -664,7 +673,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190526208"/>
+        <c:crossAx val="171321216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1042,23 +1051,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1067,6 +1079,9 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1290,7 +1305,7 @@
         <v>43982</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f>B18/C18</f>
         <v>1.0640716656814151E-2</v>
       </c>
     </row>
@@ -1388,6 +1403,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>